<commit_message>
update import script import_animals.py
</commit_message>
<xml_diff>
--- a/example_import.xlsx
+++ b/example_import.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hdinkel/repositories/anishare/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{5C0E56C4-AD97-3B42-BE00-D726688F190A}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{1A34D984-361B-BE49-9565-58C347BE7322}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="16540" xr2:uid="{5E06D273-CBFE-8A4A-9A20-2B69A48292B7}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Information exported from PYRAT:</t>
   </si>
@@ -97,6 +97,27 @@
   </si>
   <si>
     <t>New Owner</t>
+  </si>
+  <si>
+    <t>ext. ID 123</t>
+  </si>
+  <si>
+    <t>LAB123</t>
+  </si>
+  <si>
+    <t>ko/ko</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>Outside</t>
+  </si>
+  <si>
+    <t>#007</t>
+  </si>
+  <si>
+    <t>Roger Roger</t>
   </si>
 </sst>
 </file>
@@ -252,7 +273,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -299,6 +320,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -613,119 +635,160 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE3BD285-0B4D-7A44-8509-F9498D64C3C8}">
-  <dimension ref="A7:V9"/>
+  <dimension ref="A8:V11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="7" spans="1:22" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="10" t="s">
+    <row r="8" spans="1:22" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C9" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="11"/>
-      <c r="L8" s="11"/>
-      <c r="M8" s="11"/>
-      <c r="N8" s="11"/>
-      <c r="O8" s="11"/>
-      <c r="P8" s="11"/>
-      <c r="Q8" s="11"/>
-      <c r="R8" s="12"/>
-      <c r="S8" s="13" t="s">
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="11"/>
+      <c r="O9" s="11"/>
+      <c r="P9" s="11"/>
+      <c r="Q9" s="11"/>
+      <c r="R9" s="12"/>
+      <c r="S9" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="T8" s="14"/>
-      <c r="U8" s="14"/>
-      <c r="V8" s="15"/>
+      <c r="T9" s="14"/>
+      <c r="U9" s="14"/>
+      <c r="V9" s="15"/>
     </row>
-    <row r="9" spans="1:22" s="9" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+    <row r="10" spans="1:22" s="9" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D10" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E10" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="G10" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="H10" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="I9" s="5" t="s">
+      <c r="I10" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="J9" s="5" t="s">
+      <c r="J10" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="K9" s="5" t="s">
+      <c r="K10" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="L9" s="5" t="s">
+      <c r="L10" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="M9" s="5" t="s">
+      <c r="M10" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="N9" s="5" t="s">
+      <c r="N10" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="O9" s="5" t="s">
+      <c r="O10" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="P9" s="5" t="s">
+      <c r="P10" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="Q9" s="5" t="s">
+      <c r="Q10" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="R9" s="3" t="s">
+      <c r="R10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="S9" s="6" t="s">
+      <c r="S10" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="T9" s="7" t="s">
+      <c r="T10" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="U9" s="7" t="s">
+      <c r="U10" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="V9" s="8" t="s">
+      <c r="V10" s="8" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" s="16">
+        <v>43221</v>
+      </c>
+      <c r="C11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="16">
+        <v>43101</v>
+      </c>
+      <c r="F11">
+        <v>10</v>
+      </c>
+      <c r="G11" t="s">
+        <v>26</v>
+      </c>
+      <c r="P11" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>28</v>
+      </c>
+      <c r="R11" t="s">
+        <v>29</v>
+      </c>
+      <c r="S11" t="s">
+        <v>30</v>
+      </c>
+      <c r="T11" s="16">
+        <v>43252</v>
+      </c>
+      <c r="U11" s="16">
+        <v>43282</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="C8:R8"/>
-    <mergeCell ref="S8:V8"/>
+    <mergeCell ref="C9:R9"/>
+    <mergeCell ref="S9:V9"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S8:S9" xr:uid="{1E1C3154-B9B7-6042-8652-B08489FC768E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S9:S10" xr:uid="{1E1C3154-B9B7-6042-8652-B08489FC768E}">
       <formula1>#REF!</formula1>
     </dataValidation>
-    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please use a valid date (eg. 01.01.2017)" sqref="T8:U9" xr:uid="{06F8D467-2C28-0048-9CFF-1F5C92FAD4B3}">
+    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please use a valid date (eg. 01.01.2017)" sqref="T9:U10" xr:uid="{06F8D467-2C28-0048-9CFF-1F5C92FAD4B3}">
       <formula1>36526</formula1>
       <formula2>47848</formula2>
     </dataValidation>

</xml_diff>